<commit_message>
Fixed AI, added more Options
</commit_message>
<xml_diff>
--- a/Experiment_Results.xlsx
+++ b/Experiment_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\Github_Repos\Tetris-Neuroevolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C65473-DDA6-4174-90C1-3BB09B016896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E001B12B-6660-4D95-BF60-1B51D41C73BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C193979-DCE6-4835-B263-DC454A700076}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>1: Human player = false</t>
   </si>
@@ -92,13 +92,27 @@
   <si>
     <t>12: Include the tetromino's board position as an input = true</t>
   </si>
+  <si>
+    <t>Rotate</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,12 +136,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10782,10 +10814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC1A866-C794-4A4B-B6C0-3AC957B7F652}">
-  <dimension ref="A1:Q2013"/>
+  <dimension ref="A1:AD2013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10793,7 +10825,7 @@
     <col min="9" max="9" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10804,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -10815,7 +10847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -10826,7 +10858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -10837,7 +10869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -10848,7 +10880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -10858,8 +10890,11 @@
       <c r="Q6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="AB6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -10869,8 +10904,21 @@
       <c r="Q7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -10880,8 +10928,23 @@
       <c r="Q8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -10891,8 +10954,23 @@
       <c r="Q9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -10902,8 +10980,23 @@
       <c r="Q10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>8</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>9</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>10</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -10913,8 +11006,23 @@
       <c r="Q11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z11" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>12</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>13</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>14</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -10924,8 +11032,43 @@
       <c r="Q12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Y12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>16</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>17</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>18</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Z13" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>20</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>21</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>22</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -10938,8 +11081,23 @@
       <c r="Q14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z14" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>24</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>26</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -10952,8 +11110,23 @@
       <c r="Q15">
         <v>2.6666666999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z15" s="2">
+        <v>7</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>28</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>29</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -10966,8 +11139,23 @@
       <c r="Q16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z16" s="2">
+        <v>8</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>32</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>33</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>34</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -10980,8 +11168,23 @@
       <c r="Q17">
         <v>1.3333333999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Z17" s="2">
+        <v>9</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>36</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>37</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>38</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -10995,7 +11198,7 @@
         <v>2.6666666999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -11009,7 +11212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -11023,7 +11226,7 @@
         <v>1.3333333999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -11037,7 +11240,7 @@
         <v>2.6666666999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -11051,7 +11254,7 @@
         <v>1.3333333999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -11065,7 +11268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -11079,7 +11282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -11093,7 +11296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -11107,7 +11310,7 @@
         <v>2.6666666999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -11121,7 +11324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -11135,7 +11338,7 @@
         <v>2.6666666999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -11149,7 +11352,7 @@
         <v>3.3333333000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -11163,7 +11366,7 @@
         <v>2.6666666999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -11177,7 +11380,7 @@
         <v>2.6666666999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -28727,6 +28930,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>